<commit_message>
[5] Added Auction class. Working on trades.
</commit_message>
<xml_diff>
--- a/src/constants/stocks/indices_constituents_list.xlsx
+++ b/src/constants/stocks/indices_constituents_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/australien/Documents/IESEG/Master 2/Thesis/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/australien/Documents/IESEG/Master 2/Thesis/Code/src/constants/stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED542CB-2751-9948-81B3-BA9811573E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E227F91-F1E6-274D-A76B-699471391E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" firstSheet="1" activeTab="9" xr2:uid="{88EAC37D-1567-D245-820F-9EDB88DFE4B0}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="613">
   <si>
     <t>FR0000120404</t>
   </si>
@@ -1937,6 +1937,9 @@
   </si>
   <si>
     <t>liquidity_provider_program</t>
+  </si>
+  <si>
+    <t>VHOXhistory_FR0000125684_20170125 is empty</t>
   </si>
 </sst>
 </file>
@@ -3161,8 +3164,8 @@
   </sheetPr>
   <dimension ref="A1:U128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="J128" sqref="J128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,7 +3265,7 @@
       </c>
       <c r="U2">
         <f>COUNTIF(K:K, "=TRUE")</f>
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -7677,9 +7680,15 @@
       <c r="H128">
         <v>255</v>
       </c>
+      <c r="I128" t="b">
+        <v>1</v>
+      </c>
+      <c r="J128" t="s">
+        <v>612</v>
+      </c>
       <c r="K128" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>